<commit_message>
lots more images and touching up previous ones
switch to make the spritesheets with GlueIT and not manually.
</commit_message>
<xml_diff>
--- a/notes/graphic source/image numbers.xlsx
+++ b/notes/graphic source/image numbers.xlsx
@@ -49,12 +49,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,531 +402,531 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>25</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="2">
         <v>33</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="2">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="2">
         <v>34</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="2">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>35</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="2">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="2">
         <v>36</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="2">
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="2">
         <v>37</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="2">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="2">
         <v>38</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="2">
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="2">
         <v>39</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="2">
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="2">
         <v>40</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="2">
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="2">
         <v>41</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="2">
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="2">
         <v>42</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="2">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>43</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="2">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>44</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="2">
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="2">
         <v>45</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="2">
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="2">
         <v>46</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="2">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="2">
         <v>47</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="2">
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="2">
         <v>48</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="2">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start of corrected train 129+ images
</commit_message>
<xml_diff>
--- a/notes/graphic source/image numbers.xlsx
+++ b/notes/graphic source/image numbers.xlsx
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C130"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,17 +1808,6 @@
       </c>
       <c r="C129">
         <v>256</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130">
-        <v>129</v>
-      </c>
-      <c r="B130">
-        <v>129</v>
-      </c>
-      <c r="C130">
-        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redo first 16 images
</commit_message>
<xml_diff>
--- a/notes/graphic source/image numbers.xlsx
+++ b/notes/graphic source/image numbers.xlsx
@@ -31,7 +31,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,6 +48,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -58,8 +65,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -72,15 +78,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:C130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,355 +586,355 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>25</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>31</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>32</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>160</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>33</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>34</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>35</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>163</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>36</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>164</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>37</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38">
         <v>165</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <v>38</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>39</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>40</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <v>41</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <v>42</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <v>43</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46">
         <v>45</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47">
         <v>46</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47">
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48">
         <v>47</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48">
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49">
         <v>48</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some graphics continuation work
</commit_message>
<xml_diff>
--- a/notes/graphic source/image numbers.xlsx
+++ b/notes/graphic source/image numbers.xlsx
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A2:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,179 +586,179 @@
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>21</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="2">
         <v>22</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>151</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="2">
         <v>24</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="2">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="2">
         <v>25</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="2">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="2">
         <v>26</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="2">
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="2">
         <v>27</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="2">
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="2">
         <v>28</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="2">
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="2">
         <v>29</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="2">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="2">
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="2">
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <v>31</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="2">
         <v>159</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="2">
         <v>32</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="2">
         <v>160</v>
       </c>
     </row>

</xml_diff>